<commit_message>
Add COM_EMUNDUS_ONBOARD_CAMPAIGNS_AND_PROGRAMS translation, update Pinia, update composer dependencies
</commit_message>
<xml_diff>
--- a/libraries/emundus/vendor/svrnm/exceldatatables/examples/spec.xlsx
+++ b/libraries/emundus/vendor/svrnm/exceldatatables/examples/spec.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neumanns/Projects/exceldatatables/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CACA895-D423-8342-B8FF-F9A2F6789AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="687" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="1840" yWindow="880" windowWidth="16380" windowHeight="8200" tabRatio="687" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Daten" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Chart" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -30,33 +35,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,7 +53,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -76,49 +61,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -177,25 +130,46 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daten!$B$1</c:f>
+              <c:f>Data!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -205,9 +179,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
                 <a:srgbClr val="004586"/>
@@ -216,65 +187,81 @@
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="diamond"/>
             <c:size val="5"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Daten!$A$2:$A$14</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>30.07.14 00:00</c:v>
+                  <c:v>41850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.07.14 13:30</c:v>
+                  <c:v>41851.5625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>02.08.14</c:v>
+                  <c:v>41853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>03.08.14</c:v>
+                  <c:v>41854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>04.08.14</c:v>
+                  <c:v>41855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>05.08.14</c:v>
+                  <c:v>41856</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>06.08.14</c:v>
+                  <c:v>41857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>07.08.14</c:v>
+                  <c:v>41858</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>08.08.14</c:v>
+                  <c:v>41859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>09.08.14</c:v>
+                  <c:v>41860</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.08.14</c:v>
+                  <c:v>41861</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.08.14</c:v>
+                  <c:v>41862</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.08.2014 00:00:00</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41863</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daten!$B$2:$B$14</c:f>
+              <c:f>Data!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -320,13 +307,19 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB16-DD41-A0D4-1D0E3C8F4815}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daten!$C$1</c:f>
+              <c:f>Data!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -336,76 +329,89 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
+                <a:srgbClr val="FF420E"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="square"/>
             <c:size val="5"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Daten!$A$2:$A$14</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>30.07.14 00:00</c:v>
+                  <c:v>41850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.07.14 13:30</c:v>
+                  <c:v>41851.5625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>02.08.14</c:v>
+                  <c:v>41853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>03.08.14</c:v>
+                  <c:v>41854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>04.08.14</c:v>
+                  <c:v>41855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>05.08.14</c:v>
+                  <c:v>41856</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>06.08.14</c:v>
+                  <c:v>41857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>07.08.14</c:v>
+                  <c:v>41858</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>08.08.14</c:v>
+                  <c:v>41859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>09.08.14</c:v>
+                  <c:v>41860</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.08.14</c:v>
+                  <c:v>41861</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.08.14</c:v>
+                  <c:v>41862</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.08.2014 00:00:00</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41863</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daten!$C$2:$C$14</c:f>
+              <c:f>Data!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -451,8 +457,23 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BB16-DD41-A0D4-1D0E3C8F4815}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="41693387"/>
         <c:axId val="28970947"/>
       </c:lineChart>
@@ -463,13 +484,14 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -478,6 +500,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="28970947"/>
@@ -490,29 +513,31 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:crossAx val="41693387"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -528,20 +553,27 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -555,14 +587,20 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="405720" y="259200"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -575,213 +613,524 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" width="11.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Cisco Confidential</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="26.1640625"/>
+    <col min="2" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
         <v>41850</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
         <v>41851.5625</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>14</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4">
         <v>41853</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5">
         <v>41854</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6">
         <v>41855</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>23</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
         <v>41856</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>41857</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>13</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
         <v>41858</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10">
         <v>41859</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>11</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11">
         <v>41860</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>17</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12">
         <v>41861</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>41862</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13">
         <v>13</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14">
         <v>41863</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14">
         <v>44</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Cisco Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
BREAKING CHANGES: Tchooz v2
</commit_message>
<xml_diff>
--- a/libraries/emundus/vendor/svrnm/exceldatatables/examples/spec.xlsx
+++ b/libraries/emundus/vendor/svrnm/exceldatatables/examples/spec.xlsx
@@ -1,17 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <workbookPr defaultThemeVersion="202300"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/neumanns/Projects/exceldatatables/examples/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CACA895-D423-8342-B8FF-F9A2F6789AE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="687" firstSheet="0" activeTab="1"/>
+    <workbookView xWindow="1840" yWindow="880" windowWidth="16380" windowHeight="8200" tabRatio="687" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Chart" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Daten" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Chart" sheetId="1" r:id="rId1"/>
+    <sheet name="Data" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
@@ -30,33 +35,13 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -68,7 +53,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -76,49 +61,17 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
+  <cellXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
+  <cellStyles count="1">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -177,25 +130,46 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
   <c:lang val="en-US"/>
+  <c:roundedCorners val="1"/>
+  <c:style val="2"/>
   <c:chart>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
         <c:grouping val="standard"/>
+        <c:varyColors val="1"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daten!$B$1</c:f>
+              <c:f>Data!$B$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -205,9 +179,6 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="004586"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
                 <a:srgbClr val="004586"/>
@@ -216,65 +187,81 @@
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="diamond"/>
             <c:size val="5"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Daten!$A$2:$A$14</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>30.07.14 00:00</c:v>
+                  <c:v>41850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.07.14 13:30</c:v>
+                  <c:v>41851.5625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>02.08.14</c:v>
+                  <c:v>41853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>03.08.14</c:v>
+                  <c:v>41854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>04.08.14</c:v>
+                  <c:v>41855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>05.08.14</c:v>
+                  <c:v>41856</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>06.08.14</c:v>
+                  <c:v>41857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>07.08.14</c:v>
+                  <c:v>41858</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>08.08.14</c:v>
+                  <c:v>41859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>09.08.14</c:v>
+                  <c:v>41860</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.08.14</c:v>
+                  <c:v>41861</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.08.14</c:v>
+                  <c:v>41862</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.08.2014 00:00:00</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41863</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daten!$B$2:$B$14</c:f>
+              <c:f>Data!$B$2:$B$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -320,13 +307,19 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-BB16-DD41-A0D4-1D0E3C8F4815}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Daten!$C$1</c:f>
+              <c:f>Data!$C$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -336,76 +329,89 @@
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:srgbClr val="ff420e"/>
-            </a:solidFill>
             <a:ln w="28800">
               <a:solidFill>
-                <a:srgbClr val="ff420e"/>
+                <a:srgbClr val="FF420E"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
           </c:spPr>
           <c:marker>
+            <c:symbol val="square"/>
             <c:size val="5"/>
           </c:marker>
           <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
             <c:showLegendKey val="0"/>
             <c:showVal val="0"/>
             <c:showCatName val="0"/>
             <c:showSerName val="0"/>
             <c:showPercent val="0"/>
+            <c:showBubbleSize val="1"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:showLeaderLines val="0"/>
+              </c:ext>
+            </c:extLst>
           </c:dLbls>
           <c:cat>
-            <c:strRef>
-              <c:f>Daten!$A$2:$A$14</c:f>
-              <c:strCache>
+            <c:numRef>
+              <c:f>Data!$A$2:$A$14</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
                 <c:pt idx="0">
-                  <c:v>30.07.14 00:00</c:v>
+                  <c:v>41850</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>31.07.14 13:30</c:v>
+                  <c:v>41851.5625</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>02.08.14</c:v>
+                  <c:v>41853</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>03.08.14</c:v>
+                  <c:v>41854</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>04.08.14</c:v>
+                  <c:v>41855</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>05.08.14</c:v>
+                  <c:v>41856</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>06.08.14</c:v>
+                  <c:v>41857</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>07.08.14</c:v>
+                  <c:v>41858</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>08.08.14</c:v>
+                  <c:v>41859</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>09.08.14</c:v>
+                  <c:v>41860</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10.08.14</c:v>
+                  <c:v>41861</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11.08.14</c:v>
+                  <c:v>41862</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.08.2014 00:00:00</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+                  <c:v>41863</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Daten!$C$2:$C$14</c:f>
+              <c:f>Data!$C$2:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="13"/>
@@ -451,8 +457,23 @@
               </c:numCache>
             </c:numRef>
           </c:val>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-BB16-DD41-A0D4-1D0E3C8F4815}"/>
+            </c:ext>
+          </c:extLst>
         </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
         <c:marker val="1"/>
+        <c:smooth val="0"/>
         <c:axId val="41693387"/>
         <c:axId val="28970947"/>
       </c:lineChart>
@@ -463,13 +484,14 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
@@ -478,6 +500,7 @@
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="1"/>
       </c:catAx>
       <c:valAx>
         <c:axId val="28970947"/>
@@ -490,29 +513,31 @@
           <c:spPr>
             <a:ln>
               <a:solidFill>
-                <a:srgbClr val="b3b3b3"/>
+                <a:srgbClr val="B3B3B3"/>
               </a:solidFill>
             </a:ln>
           </c:spPr>
         </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:ln>
             <a:solidFill>
-              <a:srgbClr val="b3b3b3"/>
+              <a:srgbClr val="B3B3B3"/>
             </a:solidFill>
           </a:ln>
         </c:spPr>
         <c:crossAx val="41693387"/>
         <c:crossesAt val="0"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
         <a:ln>
           <a:solidFill>
-            <a:srgbClr val="b3b3b3"/>
+            <a:srgbClr val="B3B3B3"/>
           </a:solidFill>
         </a:ln>
       </c:spPr>
@@ -528,20 +553,27 @@
       </c:spPr>
     </c:legend>
     <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="1"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:srgbClr val="ffffff"/>
+      <a:srgbClr val="FFFFFF"/>
     </a:solidFill>
     <a:ln>
       <a:noFill/>
     </a:ln>
   </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
 </c:chartSpace>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
@@ -555,14 +587,20 @@
       <xdr:row>21</xdr:row>
       <xdr:rowOff>84600</xdr:rowOff>
     </xdr:to>
-    <xdr:graphicFrame>
+    <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="0" name=""/>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="405720" y="259200"/>
-        <a:ext cx="5758920" cy="3238920"/>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -575,213 +613,524 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="0E2841"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="E8E8E8"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="156082"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="E97132"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="196B24"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="0F9ED5"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="A02B93"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="4EA72E"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="467886"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="96607D"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック Light"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="游ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="等线"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="110000"/>
+                <a:satMod val="105000"/>
+                <a:tint val="67000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="103000"/>
+                <a:tint val="73000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="105000"/>
+                <a:satMod val="109000"/>
+                <a:tint val="81000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:satMod val="103000"/>
+                <a:lumMod val="102000"/>
+                <a:tint val="94000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:satMod val="110000"/>
+                <a:lumMod val="100000"/>
+                <a:shade val="100000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:lumMod val="99000"/>
+                <a:satMod val="120000"/>
+                <a:shade val="78000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst/>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="63000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:tint val="95000"/>
+            <a:satMod val="170000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="93000"/>
+                <a:satMod val="150000"/>
+                <a:shade val="98000"/>
+                <a:lumMod val="102000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="50000">
+              <a:schemeClr val="phClr">
+                <a:tint val="98000"/>
+                <a:satMod val="130000"/>
+                <a:shade val="90000"/>
+                <a:lumMod val="103000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="63000"/>
+                <a:satMod val="120000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="5400000" scaled="0"/>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults>
+    <a:lnDef>
+      <a:spPr/>
+      <a:bodyPr/>
+      <a:lstStyle/>
+      <a:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent1"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent1"/>
+        </a:fillRef>
+        <a:effectRef idx="1">
+          <a:schemeClr val="accent1"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </a:style>
+    </a:lnDef>
+  </a:objectDefaults>
+  <a:extraClrSchemeLst/>
+  <a:extLst>
+    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+    </a:ext>
+  </a:extLst>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col min="1" max="1025" width="11.5"/>
   </cols>
   <sheetData/>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" orientation="portrait" usePrinterDefaults="0" useFirstPageNumber="1" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Cisco Confidential</oddFooter>
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <sheetPr>
     <tabColor rgb="FFFFFFFF"/>
-    <pageSetUpPr fitToPage="false"/>
   </sheetPr>
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D20" activeCellId="0" sqref="D20"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.8"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="26.25"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col min="1" max="1" width="26.1640625"/>
+    <col min="2" max="1025" width="11.5"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="1" t="n">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A2">
         <v>41850</v>
       </c>
-      <c r="B2" s="0" t="n">
+      <c r="B2">
         <v>13</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2">
         <v>2</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="n">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A3">
         <v>41851.5625</v>
       </c>
-      <c r="B3" s="0" t="n">
+      <c r="B3">
         <v>14</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="C3">
         <v>4</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="1" t="n">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A4">
         <v>41853</v>
       </c>
-      <c r="B4" s="0" t="n">
+      <c r="B4">
         <v>8</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="C4">
         <v>8</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="n">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A5">
         <v>41854</v>
       </c>
-      <c r="B5" s="0" t="n">
+      <c r="B5">
         <v>9</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5">
         <v>16</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="n">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A6">
         <v>41855</v>
       </c>
-      <c r="B6" s="0" t="n">
+      <c r="B6">
         <v>23</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6">
         <v>31</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="1" t="n">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A7">
         <v>41856</v>
       </c>
-      <c r="B7" s="0" t="n">
+      <c r="B7">
         <v>11</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="C7">
         <v>25</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="1" t="n">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A8">
         <v>41857</v>
       </c>
-      <c r="B8" s="0" t="n">
+      <c r="B8">
         <v>13</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="C8">
         <v>15</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="n">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A9">
         <v>41858</v>
       </c>
-      <c r="B9" s="0" t="n">
+      <c r="B9">
         <v>18</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="C9">
         <v>10</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="n">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A10">
         <v>41859</v>
       </c>
-      <c r="B10" s="0" t="n">
+      <c r="B10">
         <v>11</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="C10">
         <v>5</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A11">
         <v>41860</v>
       </c>
-      <c r="B11" s="0" t="n">
+      <c r="B11">
         <v>17</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="C11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="1" t="n">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A12">
         <v>41861</v>
       </c>
-      <c r="B12" s="0" t="n">
+      <c r="B12">
         <v>0</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="C12">
         <v>2</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="n">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A13">
         <v>41862</v>
       </c>
-      <c r="B13" s="0" t="n">
+      <c r="B13">
         <v>13</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="C13">
         <v>0</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="n">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+      <c r="A14">
         <v>41863</v>
       </c>
-      <c r="B14" s="0" t="n">
+      <c r="B14">
         <v>44</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="C14">
         <v>33</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup paperSize="0" scale="0" firstPageNumber="0" orientation="portrait" usePrinterDefaults="0" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Standard"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P</oddFooter>
+    <oddFooter>&amp;C&amp;"Times New Roman,Standard"&amp;12Seite &amp;P&amp;R_x000D_&amp;1#&amp;"Calibri"&amp;8&amp;K000000 Cisco Confidential</oddFooter>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>